<commit_message>
📊 Update SwaadSutra_Daily_2026-01-20.xlsx - 2026-01-20T01:43:36.590Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-20.xlsx
@@ -471,7 +471,7 @@
         <v>30</v>
       </c>
       <c r="H2" t="str">
-        <v>NEW</v>
+        <v>COOKING</v>
       </c>
       <c r="I2" t="str">
         <v>PENDING</v>
@@ -537,10 +537,10 @@
         <v>1</v>
       </c>
       <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
         <v>1</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-20.xlsx - 2026-01-20T02:17:08.220Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-20.xlsx
@@ -471,7 +471,7 @@
         <v>30</v>
       </c>
       <c r="H2" t="str">
-        <v>COOKING</v>
+        <v>READY</v>
       </c>
       <c r="I2" t="str">
         <v>PENDING</v>
@@ -540,10 +540,10 @@
         <v>0</v>
       </c>
       <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
         <v>1</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
       </c>
       <c r="E2">
         <v>0</v>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-20.xlsx - 2026-01-20T02:24:49.201Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-20.xlsx
@@ -471,7 +471,7 @@
         <v>30</v>
       </c>
       <c r="H2" t="str">
-        <v>READY</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I2" t="str">
         <v>PENDING</v>
@@ -543,10 +543,10 @@
         <v>0</v>
       </c>
       <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
         <v>1</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-20.xlsx - 2026-01-20T04:28:17.508Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-20.xlsx
@@ -474,7 +474,7 @@
         <v>DELIVERED</v>
       </c>
       <c r="I2" t="str">
-        <v>PENDING</v>
+        <v>PAID</v>
       </c>
       <c r="J2" t="str">
         <v>2026-01-20</v>
@@ -555,7 +555,7 @@
         <v>30</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-20.xlsx - 2026-01-20T05:33:36.563Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-20.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,37 +450,37 @@
     </row>
     <row r="2">
       <c r="A2">
+        <v>21</v>
+      </c>
+      <c r="B2" t="str">
+        <v>2026-01-20 05:33</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D2" t="str">
+        <v>A 1608</v>
+      </c>
+      <c r="E2" t="str">
+        <v>9096648553</v>
+      </c>
+      <c r="F2" t="str">
+        <v>Jawar Bhakari x1</v>
+      </c>
+      <c r="G2">
         <v>20</v>
       </c>
-      <c r="B2" t="str">
-        <v>2026-01-20 01:42</v>
-      </c>
-      <c r="C2" t="str">
-        <v>Minakshi</v>
-      </c>
-      <c r="D2" t="str">
-        <v>A 201</v>
-      </c>
-      <c r="E2" t="str">
-        <v>7387851735</v>
-      </c>
-      <c r="F2" t="str">
-        <v>Wheat Chapati x2</v>
-      </c>
-      <c r="G2">
-        <v>30</v>
-      </c>
       <c r="H2" t="str">
-        <v>DELIVERED</v>
+        <v>NEW</v>
       </c>
       <c r="I2" t="str">
-        <v>PAID</v>
+        <v>PENDING</v>
       </c>
       <c r="J2" t="str">
         <v>2026-01-20</v>
       </c>
       <c r="K2" t="str">
-        <v>08:00</v>
+        <v>11:03</v>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -492,9 +492,53 @@
         <v/>
       </c>
     </row>
+    <row r="3">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3" t="str">
+        <v>2026-01-20 01:42</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Minakshi</v>
+      </c>
+      <c r="D3" t="str">
+        <v>A 201</v>
+      </c>
+      <c r="E3" t="str">
+        <v>7387851735</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Wheat Chapati x2</v>
+      </c>
+      <c r="G3">
+        <v>30</v>
+      </c>
+      <c r="H3" t="str">
+        <v>DELIVERED</v>
+      </c>
+      <c r="I3" t="str">
+        <v>PAID</v>
+      </c>
+      <c r="J3" t="str">
+        <v>2026-01-20</v>
+      </c>
+      <c r="K3" t="str">
+        <v>08:00</v>
+      </c>
+      <c r="L3" t="str">
+        <v/>
+      </c>
+      <c r="M3" t="str">
+        <v/>
+      </c>
+      <c r="N3" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N3"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -534,10 +578,10 @@
     </row>
     <row r="2">
       <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
         <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -552,7 +596,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H2">
         <v>30</v>
@@ -567,7 +611,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -594,9 +638,20 @@
         <v>30</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Jawar Bhakari</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-20.xlsx - 2026-01-20T05:33:51.267Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-20.xlsx
@@ -471,7 +471,7 @@
         <v>20</v>
       </c>
       <c r="H2" t="str">
-        <v>NEW</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I2" t="str">
         <v>PENDING</v>
@@ -581,7 +581,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2">
         <v>0</v>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-20.xlsx - 2026-01-20T05:33:55.996Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-20.xlsx
@@ -474,7 +474,7 @@
         <v>DELIVERED</v>
       </c>
       <c r="I2" t="str">
-        <v>PENDING</v>
+        <v>PAID</v>
       </c>
       <c r="J2" t="str">
         <v>2026-01-20</v>
@@ -599,7 +599,7 @@
         <v>50</v>
       </c>
       <c r="H2">
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-20.xlsx - 2026-01-20T11:13:38.635Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-20.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,37 +450,37 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-20 05:33</v>
+        <v>2026-01-20 11:13</v>
       </c>
       <c r="C2" t="str">
         <v>Pooja</v>
       </c>
       <c r="D2" t="str">
-        <v>A 1608</v>
+        <v>12</v>
       </c>
       <c r="E2" t="str">
         <v>9096648553</v>
       </c>
       <c r="F2" t="str">
-        <v>Jawar Bhakari x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H2" t="str">
-        <v>DELIVERED</v>
+        <v>NEW</v>
       </c>
       <c r="I2" t="str">
-        <v>PAID</v>
+        <v>PENDING</v>
       </c>
       <c r="J2" t="str">
         <v>2026-01-20</v>
       </c>
       <c r="K2" t="str">
-        <v>11:03</v>
+        <v>16:43</v>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -494,25 +494,25 @@
     </row>
     <row r="3">
       <c r="A3">
+        <v>21</v>
+      </c>
+      <c r="B3" t="str">
+        <v>2026-01-20 05:33</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D3" t="str">
+        <v>A 1608</v>
+      </c>
+      <c r="E3" t="str">
+        <v>9096648553</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Jawar Bhakari x1</v>
+      </c>
+      <c r="G3">
         <v>20</v>
-      </c>
-      <c r="B3" t="str">
-        <v>2026-01-20 01:42</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Minakshi</v>
-      </c>
-      <c r="D3" t="str">
-        <v>A 201</v>
-      </c>
-      <c r="E3" t="str">
-        <v>7387851735</v>
-      </c>
-      <c r="F3" t="str">
-        <v>Wheat Chapati x2</v>
-      </c>
-      <c r="G3">
-        <v>30</v>
       </c>
       <c r="H3" t="str">
         <v>DELIVERED</v>
@@ -524,21 +524,65 @@
         <v>2026-01-20</v>
       </c>
       <c r="K3" t="str">
+        <v>11:03</v>
+      </c>
+      <c r="L3" t="str">
+        <v/>
+      </c>
+      <c r="M3" t="str">
+        <v/>
+      </c>
+      <c r="N3" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>20</v>
+      </c>
+      <c r="B4" t="str">
+        <v>2026-01-20 01:42</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Minakshi</v>
+      </c>
+      <c r="D4" t="str">
+        <v>A 201</v>
+      </c>
+      <c r="E4" t="str">
+        <v>7387851735</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Wheat Chapati x2</v>
+      </c>
+      <c r="G4">
+        <v>30</v>
+      </c>
+      <c r="H4" t="str">
+        <v>DELIVERED</v>
+      </c>
+      <c r="I4" t="str">
+        <v>PAID</v>
+      </c>
+      <c r="J4" t="str">
+        <v>2026-01-20</v>
+      </c>
+      <c r="K4" t="str">
         <v>08:00</v>
       </c>
-      <c r="L3" t="str">
-        <v/>
-      </c>
-      <c r="M3" t="str">
-        <v/>
-      </c>
-      <c r="N3" t="str">
+      <c r="L4" t="str">
+        <v/>
+      </c>
+      <c r="M4" t="str">
+        <v/>
+      </c>
+      <c r="N4" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N4"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -578,10 +622,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -596,7 +640,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="H2">
         <v>50</v>
@@ -611,7 +655,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -640,18 +684,29 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Jawar Bhakari</v>
+        <v>Til Poli</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Jawar Bhakari</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-20.xlsx - 2026-01-20T11:14:10.525Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-20.xlsx
@@ -471,7 +471,7 @@
         <v>30</v>
       </c>
       <c r="H2" t="str">
-        <v>NEW</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I2" t="str">
         <v>PENDING</v>
@@ -625,7 +625,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -634,7 +634,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2">
         <v>0</v>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-20.xlsx - 2026-01-20T12:17:30.277Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-20.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,37 +450,37 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-20 11:13</v>
+        <v>2026-01-20 12:17</v>
       </c>
       <c r="C2" t="str">
-        <v>Pooja</v>
+        <v>Radha shelke</v>
       </c>
       <c r="D2" t="str">
-        <v>12</v>
+        <v>C 803</v>
       </c>
       <c r="E2" t="str">
-        <v>9096648553</v>
+        <v>9890774770</v>
       </c>
       <c r="F2" t="str">
-        <v>Til Poli x1</v>
+        <v>Appe Chutney x2, Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G2">
-        <v>30</v>
+        <v>180</v>
       </c>
       <c r="H2" t="str">
-        <v>DELIVERED</v>
+        <v>NEW</v>
       </c>
       <c r="I2" t="str">
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v>2026-01-20</v>
+        <v/>
       </c>
       <c r="K2" t="str">
-        <v>16:43</v>
+        <v/>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -494,37 +494,37 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-20 05:33</v>
+        <v>2026-01-20 11:13</v>
       </c>
       <c r="C3" t="str">
         <v>Pooja</v>
       </c>
       <c r="D3" t="str">
-        <v>A 1608</v>
+        <v>12</v>
       </c>
       <c r="E3" t="str">
         <v>9096648553</v>
       </c>
       <c r="F3" t="str">
-        <v>Jawar Bhakari x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G3">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H3" t="str">
         <v>DELIVERED</v>
       </c>
       <c r="I3" t="str">
-        <v>PAID</v>
+        <v>PENDING</v>
       </c>
       <c r="J3" t="str">
         <v>2026-01-20</v>
       </c>
       <c r="K3" t="str">
-        <v>11:03</v>
+        <v>16:43</v>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -538,25 +538,25 @@
     </row>
     <row r="4">
       <c r="A4">
+        <v>21</v>
+      </c>
+      <c r="B4" t="str">
+        <v>2026-01-20 05:33</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D4" t="str">
+        <v>A 1608</v>
+      </c>
+      <c r="E4" t="str">
+        <v>9096648553</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Jawar Bhakari x1</v>
+      </c>
+      <c r="G4">
         <v>20</v>
-      </c>
-      <c r="B4" t="str">
-        <v>2026-01-20 01:42</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Minakshi</v>
-      </c>
-      <c r="D4" t="str">
-        <v>A 201</v>
-      </c>
-      <c r="E4" t="str">
-        <v>7387851735</v>
-      </c>
-      <c r="F4" t="str">
-        <v>Wheat Chapati x2</v>
-      </c>
-      <c r="G4">
-        <v>30</v>
       </c>
       <c r="H4" t="str">
         <v>DELIVERED</v>
@@ -568,21 +568,65 @@
         <v>2026-01-20</v>
       </c>
       <c r="K4" t="str">
+        <v>11:03</v>
+      </c>
+      <c r="L4" t="str">
+        <v/>
+      </c>
+      <c r="M4" t="str">
+        <v/>
+      </c>
+      <c r="N4" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>20</v>
+      </c>
+      <c r="B5" t="str">
+        <v>2026-01-20 01:42</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Minakshi</v>
+      </c>
+      <c r="D5" t="str">
+        <v>A 201</v>
+      </c>
+      <c r="E5" t="str">
+        <v>7387851735</v>
+      </c>
+      <c r="F5" t="str">
+        <v>Wheat Chapati x2</v>
+      </c>
+      <c r="G5">
+        <v>30</v>
+      </c>
+      <c r="H5" t="str">
+        <v>DELIVERED</v>
+      </c>
+      <c r="I5" t="str">
+        <v>PAID</v>
+      </c>
+      <c r="J5" t="str">
+        <v>2026-01-20</v>
+      </c>
+      <c r="K5" t="str">
         <v>08:00</v>
       </c>
-      <c r="L4" t="str">
-        <v/>
-      </c>
-      <c r="M4" t="str">
-        <v/>
-      </c>
-      <c r="N4" t="str">
+      <c r="L5" t="str">
+        <v/>
+      </c>
+      <c r="M5" t="str">
+        <v/>
+      </c>
+      <c r="N5" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N5"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -622,10 +666,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -640,7 +684,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>80</v>
+        <v>260</v>
       </c>
       <c r="H2">
         <v>50</v>
@@ -655,7 +699,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -673,21 +717,21 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Wheat Chapati</v>
+        <v>Appe Chutney</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
       <c r="C2">
-        <v>30</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Til Poli</v>
+        <v>Wheat Chapati</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>30</v>
@@ -695,18 +739,40 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Jawar Bhakari</v>
+        <v>Onion Pakoda (Kanda Bhaje)</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Til Poli</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Jawar Bhakari</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-20.xlsx - 2026-01-20T15:03:45.974Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-20.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,25 +450,25 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-20 12:17</v>
+        <v>2026-01-20 15:03</v>
       </c>
       <c r="C2" t="str">
-        <v>Radha shelke</v>
+        <v>Udita Roy</v>
       </c>
       <c r="D2" t="str">
-        <v>C 803</v>
+        <v>A-1603</v>
       </c>
       <c r="E2" t="str">
-        <v>9890774770</v>
+        <v>7061856166</v>
       </c>
       <c r="F2" t="str">
-        <v>Appe Chutney x2, Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Appe Chutney x1</v>
       </c>
       <c r="G2">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -477,13 +477,13 @@
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v/>
+        <v>2026-01-21</v>
       </c>
       <c r="K2" t="str">
-        <v/>
+        <v>09:30</v>
       </c>
       <c r="L2" t="str">
-        <v/>
+        <v>Less spicy. Flavourful</v>
       </c>
       <c r="M2" t="str">
         <v/>
@@ -494,37 +494,37 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-20 11:13</v>
+        <v>2026-01-20 12:17</v>
       </c>
       <c r="C3" t="str">
-        <v>Pooja</v>
+        <v>Radha shelke</v>
       </c>
       <c r="D3" t="str">
-        <v>12</v>
+        <v>C 803</v>
       </c>
       <c r="E3" t="str">
-        <v>9096648553</v>
+        <v>9890774770</v>
       </c>
       <c r="F3" t="str">
-        <v>Til Poli x1</v>
+        <v>Appe Chutney x2, Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G3">
-        <v>30</v>
+        <v>180</v>
       </c>
       <c r="H3" t="str">
-        <v>DELIVERED</v>
+        <v>NEW</v>
       </c>
       <c r="I3" t="str">
         <v>PENDING</v>
       </c>
       <c r="J3" t="str">
-        <v>2026-01-20</v>
+        <v/>
       </c>
       <c r="K3" t="str">
-        <v>16:43</v>
+        <v/>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -538,37 +538,37 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-20 05:33</v>
+        <v>2026-01-20 11:13</v>
       </c>
       <c r="C4" t="str">
         <v>Pooja</v>
       </c>
       <c r="D4" t="str">
-        <v>A 1608</v>
+        <v>12</v>
       </c>
       <c r="E4" t="str">
         <v>9096648553</v>
       </c>
       <c r="F4" t="str">
-        <v>Jawar Bhakari x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G4">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H4" t="str">
         <v>DELIVERED</v>
       </c>
       <c r="I4" t="str">
-        <v>PAID</v>
+        <v>PENDING</v>
       </c>
       <c r="J4" t="str">
         <v>2026-01-20</v>
       </c>
       <c r="K4" t="str">
-        <v>11:03</v>
+        <v>16:43</v>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -582,25 +582,25 @@
     </row>
     <row r="5">
       <c r="A5">
+        <v>21</v>
+      </c>
+      <c r="B5" t="str">
+        <v>2026-01-20 05:33</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D5" t="str">
+        <v>A 1608</v>
+      </c>
+      <c r="E5" t="str">
+        <v>9096648553</v>
+      </c>
+      <c r="F5" t="str">
+        <v>Jawar Bhakari x1</v>
+      </c>
+      <c r="G5">
         <v>20</v>
-      </c>
-      <c r="B5" t="str">
-        <v>2026-01-20 01:42</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Minakshi</v>
-      </c>
-      <c r="D5" t="str">
-        <v>A 201</v>
-      </c>
-      <c r="E5" t="str">
-        <v>7387851735</v>
-      </c>
-      <c r="F5" t="str">
-        <v>Wheat Chapati x2</v>
-      </c>
-      <c r="G5">
-        <v>30</v>
       </c>
       <c r="H5" t="str">
         <v>DELIVERED</v>
@@ -612,21 +612,65 @@
         <v>2026-01-20</v>
       </c>
       <c r="K5" t="str">
+        <v>11:03</v>
+      </c>
+      <c r="L5" t="str">
+        <v/>
+      </c>
+      <c r="M5" t="str">
+        <v/>
+      </c>
+      <c r="N5" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>20</v>
+      </c>
+      <c r="B6" t="str">
+        <v>2026-01-20 01:42</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Minakshi</v>
+      </c>
+      <c r="D6" t="str">
+        <v>A 201</v>
+      </c>
+      <c r="E6" t="str">
+        <v>7387851735</v>
+      </c>
+      <c r="F6" t="str">
+        <v>Wheat Chapati x2</v>
+      </c>
+      <c r="G6">
+        <v>30</v>
+      </c>
+      <c r="H6" t="str">
+        <v>DELIVERED</v>
+      </c>
+      <c r="I6" t="str">
+        <v>PAID</v>
+      </c>
+      <c r="J6" t="str">
+        <v>2026-01-20</v>
+      </c>
+      <c r="K6" t="str">
         <v>08:00</v>
       </c>
-      <c r="L5" t="str">
-        <v/>
-      </c>
-      <c r="M5" t="str">
-        <v/>
-      </c>
-      <c r="N5" t="str">
+      <c r="L6" t="str">
+        <v/>
+      </c>
+      <c r="M6" t="str">
+        <v/>
+      </c>
+      <c r="N6" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N6"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -666,10 +710,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -684,7 +728,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>260</v>
+        <v>320</v>
       </c>
       <c r="H2">
         <v>50</v>
@@ -720,10 +764,10 @@
         <v>Appe Chutney</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2">
-        <v>120</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-20.xlsx - 2026-01-20T15:05:10.548Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-20.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,19 +450,19 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-20 15:03</v>
+        <v>2026-01-20 15:05</v>
       </c>
       <c r="C2" t="str">
-        <v>Udita Roy</v>
+        <v>Indrani Karmakar</v>
       </c>
       <c r="D2" t="str">
-        <v>A-1603</v>
+        <v>A-1903</v>
       </c>
       <c r="E2" t="str">
-        <v>7061856166</v>
+        <v>7030961520</v>
       </c>
       <c r="F2" t="str">
         <v>Appe Chutney x1</v>
@@ -480,7 +480,7 @@
         <v>2026-01-21</v>
       </c>
       <c r="K2" t="str">
-        <v>09:30</v>
+        <v>09:00</v>
       </c>
       <c r="L2" t="str">
         <v>Less spicy. Flavourful</v>
@@ -494,25 +494,25 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-20 12:17</v>
+        <v>2026-01-20 15:03</v>
       </c>
       <c r="C3" t="str">
-        <v>Radha shelke</v>
+        <v>Udita Roy</v>
       </c>
       <c r="D3" t="str">
-        <v>C 803</v>
+        <v>A-1603</v>
       </c>
       <c r="E3" t="str">
-        <v>9890774770</v>
+        <v>7061856166</v>
       </c>
       <c r="F3" t="str">
-        <v>Appe Chutney x2, Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Appe Chutney x1</v>
       </c>
       <c r="G3">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="H3" t="str">
         <v>NEW</v>
@@ -521,13 +521,13 @@
         <v>PENDING</v>
       </c>
       <c r="J3" t="str">
-        <v/>
+        <v>2026-01-21</v>
       </c>
       <c r="K3" t="str">
-        <v/>
+        <v>09:30</v>
       </c>
       <c r="L3" t="str">
-        <v/>
+        <v>Less spicy. Flavourful</v>
       </c>
       <c r="M3" t="str">
         <v/>
@@ -538,37 +538,37 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-20 11:13</v>
+        <v>2026-01-20 12:17</v>
       </c>
       <c r="C4" t="str">
-        <v>Pooja</v>
+        <v>Radha shelke</v>
       </c>
       <c r="D4" t="str">
-        <v>12</v>
+        <v>C 803</v>
       </c>
       <c r="E4" t="str">
-        <v>9096648553</v>
+        <v>9890774770</v>
       </c>
       <c r="F4" t="str">
-        <v>Til Poli x1</v>
+        <v>Appe Chutney x2, Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G4">
-        <v>30</v>
+        <v>180</v>
       </c>
       <c r="H4" t="str">
-        <v>DELIVERED</v>
+        <v>NEW</v>
       </c>
       <c r="I4" t="str">
         <v>PENDING</v>
       </c>
       <c r="J4" t="str">
-        <v>2026-01-20</v>
+        <v/>
       </c>
       <c r="K4" t="str">
-        <v>16:43</v>
+        <v/>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -582,37 +582,37 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-20 05:33</v>
+        <v>2026-01-20 11:13</v>
       </c>
       <c r="C5" t="str">
         <v>Pooja</v>
       </c>
       <c r="D5" t="str">
-        <v>A 1608</v>
+        <v>12</v>
       </c>
       <c r="E5" t="str">
         <v>9096648553</v>
       </c>
       <c r="F5" t="str">
-        <v>Jawar Bhakari x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G5">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H5" t="str">
         <v>DELIVERED</v>
       </c>
       <c r="I5" t="str">
-        <v>PAID</v>
+        <v>PENDING</v>
       </c>
       <c r="J5" t="str">
         <v>2026-01-20</v>
       </c>
       <c r="K5" t="str">
-        <v>11:03</v>
+        <v>16:43</v>
       </c>
       <c r="L5" t="str">
         <v/>
@@ -626,25 +626,25 @@
     </row>
     <row r="6">
       <c r="A6">
+        <v>21</v>
+      </c>
+      <c r="B6" t="str">
+        <v>2026-01-20 05:33</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D6" t="str">
+        <v>A 1608</v>
+      </c>
+      <c r="E6" t="str">
+        <v>9096648553</v>
+      </c>
+      <c r="F6" t="str">
+        <v>Jawar Bhakari x1</v>
+      </c>
+      <c r="G6">
         <v>20</v>
-      </c>
-      <c r="B6" t="str">
-        <v>2026-01-20 01:42</v>
-      </c>
-      <c r="C6" t="str">
-        <v>Minakshi</v>
-      </c>
-      <c r="D6" t="str">
-        <v>A 201</v>
-      </c>
-      <c r="E6" t="str">
-        <v>7387851735</v>
-      </c>
-      <c r="F6" t="str">
-        <v>Wheat Chapati x2</v>
-      </c>
-      <c r="G6">
-        <v>30</v>
       </c>
       <c r="H6" t="str">
         <v>DELIVERED</v>
@@ -656,21 +656,65 @@
         <v>2026-01-20</v>
       </c>
       <c r="K6" t="str">
+        <v>11:03</v>
+      </c>
+      <c r="L6" t="str">
+        <v/>
+      </c>
+      <c r="M6" t="str">
+        <v/>
+      </c>
+      <c r="N6" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>20</v>
+      </c>
+      <c r="B7" t="str">
+        <v>2026-01-20 01:42</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Minakshi</v>
+      </c>
+      <c r="D7" t="str">
+        <v>A 201</v>
+      </c>
+      <c r="E7" t="str">
+        <v>7387851735</v>
+      </c>
+      <c r="F7" t="str">
+        <v>Wheat Chapati x2</v>
+      </c>
+      <c r="G7">
+        <v>30</v>
+      </c>
+      <c r="H7" t="str">
+        <v>DELIVERED</v>
+      </c>
+      <c r="I7" t="str">
+        <v>PAID</v>
+      </c>
+      <c r="J7" t="str">
+        <v>2026-01-20</v>
+      </c>
+      <c r="K7" t="str">
         <v>08:00</v>
       </c>
-      <c r="L6" t="str">
-        <v/>
-      </c>
-      <c r="M6" t="str">
-        <v/>
-      </c>
-      <c r="N6" t="str">
+      <c r="L7" t="str">
+        <v/>
+      </c>
+      <c r="M7" t="str">
+        <v/>
+      </c>
+      <c r="N7" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N7"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -710,10 +754,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -728,7 +772,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>320</v>
+        <v>380</v>
       </c>
       <c r="H2">
         <v>50</v>
@@ -764,10 +808,10 @@
         <v>Appe Chutney</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>180</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-20.xlsx - 2026-01-20T16:17:59.061Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-20.xlsx
@@ -518,7 +518,7 @@
         <v>NEW</v>
       </c>
       <c r="I3" t="str">
-        <v>PENDING</v>
+        <v>PAID</v>
       </c>
       <c r="J3" t="str">
         <v>2026-01-21</v>
@@ -775,7 +775,7 @@
         <v>380</v>
       </c>
       <c r="H2">
-        <v>50</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-20.xlsx - 2026-01-20T17:36:49.512Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-20.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-20.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,25 +450,25 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-20 15:05</v>
+        <v>2026-01-20 17:36</v>
       </c>
       <c r="C2" t="str">
-        <v>Indrani Karmakar</v>
+        <v>Priyanka Patil</v>
       </c>
       <c r="D2" t="str">
-        <v>A-1903</v>
+        <v>A-1605</v>
       </c>
       <c r="E2" t="str">
-        <v>7030961520</v>
+        <v>9867003224</v>
       </c>
       <c r="F2" t="str">
-        <v>Appe Chutney x1</v>
+        <v>Appe Chutney x2</v>
       </c>
       <c r="G2">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -480,10 +480,10 @@
         <v>2026-01-21</v>
       </c>
       <c r="K2" t="str">
-        <v>09:00</v>
+        <v>09:15</v>
       </c>
       <c r="L2" t="str">
-        <v>Less spicy. Flavourful</v>
+        <v/>
       </c>
       <c r="M2" t="str">
         <v/>
@@ -494,19 +494,19 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-20 15:03</v>
+        <v>2026-01-20 15:05</v>
       </c>
       <c r="C3" t="str">
-        <v>Udita Roy</v>
+        <v>Indrani Karmakar</v>
       </c>
       <c r="D3" t="str">
-        <v>A-1603</v>
+        <v>A-1903</v>
       </c>
       <c r="E3" t="str">
-        <v>7061856166</v>
+        <v>7030961520</v>
       </c>
       <c r="F3" t="str">
         <v>Appe Chutney x1</v>
@@ -524,7 +524,7 @@
         <v>2026-01-21</v>
       </c>
       <c r="K3" t="str">
-        <v>09:30</v>
+        <v>09:00</v>
       </c>
       <c r="L3" t="str">
         <v>Less spicy. Flavourful</v>
@@ -538,40 +538,40 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-20 12:17</v>
+        <v>2026-01-20 15:03</v>
       </c>
       <c r="C4" t="str">
-        <v>Radha shelke</v>
+        <v>Udita Roy</v>
       </c>
       <c r="D4" t="str">
-        <v>C 803</v>
+        <v>A-1603</v>
       </c>
       <c r="E4" t="str">
-        <v>9890774770</v>
+        <v>7061856166</v>
       </c>
       <c r="F4" t="str">
-        <v>Appe Chutney x2, Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Appe Chutney x1</v>
       </c>
       <c r="G4">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="H4" t="str">
         <v>NEW</v>
       </c>
       <c r="I4" t="str">
-        <v>PENDING</v>
+        <v>PAID</v>
       </c>
       <c r="J4" t="str">
-        <v/>
+        <v>2026-01-21</v>
       </c>
       <c r="K4" t="str">
-        <v/>
+        <v>09:30</v>
       </c>
       <c r="L4" t="str">
-        <v/>
+        <v>Less spicy. Flavourful</v>
       </c>
       <c r="M4" t="str">
         <v/>
@@ -582,37 +582,37 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-20 11:13</v>
+        <v>2026-01-20 12:17</v>
       </c>
       <c r="C5" t="str">
-        <v>Pooja</v>
+        <v>Radha shelke</v>
       </c>
       <c r="D5" t="str">
-        <v>12</v>
+        <v>C 803</v>
       </c>
       <c r="E5" t="str">
-        <v>9096648553</v>
+        <v>9890774770</v>
       </c>
       <c r="F5" t="str">
-        <v>Til Poli x1</v>
+        <v>Appe Chutney x2, Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G5">
-        <v>30</v>
+        <v>180</v>
       </c>
       <c r="H5" t="str">
-        <v>DELIVERED</v>
+        <v>NEW</v>
       </c>
       <c r="I5" t="str">
         <v>PENDING</v>
       </c>
       <c r="J5" t="str">
-        <v>2026-01-20</v>
+        <v/>
       </c>
       <c r="K5" t="str">
-        <v>16:43</v>
+        <v/>
       </c>
       <c r="L5" t="str">
         <v/>
@@ -626,37 +626,37 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-20 05:33</v>
+        <v>2026-01-20 11:13</v>
       </c>
       <c r="C6" t="str">
         <v>Pooja</v>
       </c>
       <c r="D6" t="str">
-        <v>A 1608</v>
+        <v>12</v>
       </c>
       <c r="E6" t="str">
         <v>9096648553</v>
       </c>
       <c r="F6" t="str">
-        <v>Jawar Bhakari x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G6">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H6" t="str">
         <v>DELIVERED</v>
       </c>
       <c r="I6" t="str">
-        <v>PAID</v>
+        <v>PENDING</v>
       </c>
       <c r="J6" t="str">
         <v>2026-01-20</v>
       </c>
       <c r="K6" t="str">
-        <v>11:03</v>
+        <v>16:43</v>
       </c>
       <c r="L6" t="str">
         <v/>
@@ -670,25 +670,25 @@
     </row>
     <row r="7">
       <c r="A7">
+        <v>21</v>
+      </c>
+      <c r="B7" t="str">
+        <v>2026-01-20 05:33</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D7" t="str">
+        <v>A 1608</v>
+      </c>
+      <c r="E7" t="str">
+        <v>9096648553</v>
+      </c>
+      <c r="F7" t="str">
+        <v>Jawar Bhakari x1</v>
+      </c>
+      <c r="G7">
         <v>20</v>
-      </c>
-      <c r="B7" t="str">
-        <v>2026-01-20 01:42</v>
-      </c>
-      <c r="C7" t="str">
-        <v>Minakshi</v>
-      </c>
-      <c r="D7" t="str">
-        <v>A 201</v>
-      </c>
-      <c r="E7" t="str">
-        <v>7387851735</v>
-      </c>
-      <c r="F7" t="str">
-        <v>Wheat Chapati x2</v>
-      </c>
-      <c r="G7">
-        <v>30</v>
       </c>
       <c r="H7" t="str">
         <v>DELIVERED</v>
@@ -700,21 +700,65 @@
         <v>2026-01-20</v>
       </c>
       <c r="K7" t="str">
+        <v>11:03</v>
+      </c>
+      <c r="L7" t="str">
+        <v/>
+      </c>
+      <c r="M7" t="str">
+        <v/>
+      </c>
+      <c r="N7" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>20</v>
+      </c>
+      <c r="B8" t="str">
+        <v>2026-01-20 01:42</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Minakshi</v>
+      </c>
+      <c r="D8" t="str">
+        <v>A 201</v>
+      </c>
+      <c r="E8" t="str">
+        <v>7387851735</v>
+      </c>
+      <c r="F8" t="str">
+        <v>Wheat Chapati x2</v>
+      </c>
+      <c r="G8">
+        <v>30</v>
+      </c>
+      <c r="H8" t="str">
+        <v>DELIVERED</v>
+      </c>
+      <c r="I8" t="str">
+        <v>PAID</v>
+      </c>
+      <c r="J8" t="str">
+        <v>2026-01-20</v>
+      </c>
+      <c r="K8" t="str">
         <v>08:00</v>
       </c>
-      <c r="L7" t="str">
-        <v/>
-      </c>
-      <c r="M7" t="str">
-        <v/>
-      </c>
-      <c r="N7" t="str">
+      <c r="L8" t="str">
+        <v/>
+      </c>
+      <c r="M8" t="str">
+        <v/>
+      </c>
+      <c r="N8" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N8"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -754,10 +798,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -772,10 +816,10 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>380</v>
+        <v>500</v>
       </c>
       <c r="H2">
-        <v>110</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -808,10 +852,10 @@
         <v>Appe Chutney</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2">
-        <v>240</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3">

</xml_diff>